<commit_message>
Left weight and duplicate entries formatting
</commit_message>
<xml_diff>
--- a/resources/dhl_csv_headers.xlsx
+++ b/resources/dhl_csv_headers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Clement\Documents\GitHub\shopify-to-dhl-orders\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89817021-E4DF-4D89-9CFE-DAB57E645F37}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6C2B97-6FCB-4305-9BC4-41441D622003}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42435" yWindow="4095" windowWidth="23700" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -662,13 +662,103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DB1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="26" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="19" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="53" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="19" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="65" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="12" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="72" max="76" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="77" max="78" width="20" bestFit="1" customWidth="1"/>
+    <col min="79" max="80" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="83" max="84" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="15" bestFit="1" customWidth="1"/>
+    <col min="92" max="93" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="12" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="20" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:106" x14ac:dyDescent="0.25">

</xml_diff>